<commit_message>
Made changes to UI and acronym search
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Programming\Python Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5755972C-E261-4C64-8B63-EFCA1F5DB1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F788AAF9-E0C1-4C8C-AF72-D47C37B8B797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Updates" sheetId="5" r:id="rId1"/>
@@ -3574,6 +3574,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3583,91 +3613,61 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3952,7 +3952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825AAD22-E8D8-45EA-B8B8-D05372AA537B}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -6619,10 +6619,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F53C648C-CF69-4139-886D-FC43B831BDB6}">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B17"/>
+    <sheetView tabSelected="1" topLeftCell="C103" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -6653,129 +6653,129 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="143" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="144" t="s">
+      <c r="B2" s="117" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="128" t="s">
         <v>92</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="141"/>
+      <c r="E2" s="113"/>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
-      <c r="B3" s="126"/>
-      <c r="C3" s="115"/>
+      <c r="A3" s="116"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="125"/>
       <c r="D3" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="128"/>
+      <c r="E3" s="114"/>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="113" t="s">
+      <c r="B4" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="123" t="s">
         <v>95</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="127"/>
+      <c r="E4" s="126"/>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="123"/>
-      <c r="B5" s="125"/>
-      <c r="C5" s="114"/>
+      <c r="A5" s="120"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="124"/>
       <c r="D5" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="129"/>
+      <c r="E5" s="127"/>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="123"/>
-      <c r="B6" s="125"/>
-      <c r="C6" s="114"/>
+      <c r="A6" s="120"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="124"/>
       <c r="D6" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="129"/>
+      <c r="E6" s="127"/>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="124"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="115"/>
+      <c r="A7" s="116"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="125"/>
       <c r="D7" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="128"/>
+      <c r="E7" s="114"/>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="113" t="s">
+      <c r="B8" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="123" t="s">
         <v>100</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="127"/>
+      <c r="E8" s="126"/>
     </row>
     <row r="9" spans="1:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
-      <c r="B9" s="126"/>
-      <c r="C9" s="115"/>
+      <c r="A9" s="116"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="125"/>
       <c r="D9" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="128"/>
+      <c r="E9" s="114"/>
     </row>
     <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="113" t="s">
+      <c r="B10" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="123" t="s">
         <v>103</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="113" t="s">
+      <c r="E10" s="123" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
-      <c r="B11" s="126"/>
-      <c r="C11" s="115"/>
+      <c r="A11" s="116"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="125"/>
       <c r="D11" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="115"/>
+      <c r="E11" s="125"/>
     </row>
     <row r="12" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="113" t="s">
+      <c r="B12" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="123" t="s">
         <v>107</v>
       </c>
       <c r="D12" s="14" t="s">
@@ -6786,9 +6786,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="123"/>
-      <c r="B13" s="125"/>
-      <c r="C13" s="114"/>
+      <c r="A13" s="120"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="124"/>
       <c r="D13" s="15" t="s">
         <v>109</v>
       </c>
@@ -6797,9 +6797,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="123"/>
-      <c r="B14" s="125"/>
-      <c r="C14" s="114"/>
+      <c r="A14" s="120"/>
+      <c r="B14" s="122"/>
+      <c r="C14" s="124"/>
       <c r="D14" s="15" t="s">
         <v>110</v>
       </c>
@@ -6808,9 +6808,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="123"/>
-      <c r="B15" s="125"/>
-      <c r="C15" s="114"/>
+      <c r="A15" s="120"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="124"/>
       <c r="D15" s="15" t="s">
         <v>111</v>
       </c>
@@ -6819,64 +6819,64 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="123"/>
-      <c r="B16" s="125"/>
-      <c r="C16" s="114"/>
+      <c r="A16" s="120"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="124"/>
       <c r="D16" s="15" t="s">
         <v>112</v>
       </c>
       <c r="E16" s="33"/>
     </row>
     <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="124"/>
-      <c r="B17" s="126"/>
-      <c r="C17" s="115"/>
+      <c r="A17" s="116"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="125"/>
       <c r="D17" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="116" t="s">
+      <c r="A18" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="113" t="s">
+      <c r="B18" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="123" t="s">
         <v>118</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E18" s="121"/>
+      <c r="E18" s="129"/>
     </row>
     <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="123"/>
-      <c r="B19" s="125"/>
-      <c r="C19" s="114"/>
+      <c r="A19" s="120"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="124"/>
       <c r="D19" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E19" s="131"/>
+      <c r="E19" s="130"/>
     </row>
     <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="124"/>
-      <c r="B20" s="126"/>
-      <c r="C20" s="115"/>
+      <c r="A20" s="116"/>
+      <c r="B20" s="118"/>
+      <c r="C20" s="125"/>
       <c r="D20" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E20" s="130"/>
+      <c r="E20" s="131"/>
     </row>
     <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="113" t="s">
+      <c r="B21" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="123" t="s">
         <v>122</v>
       </c>
       <c r="D21" s="14" t="s">
@@ -6887,9 +6887,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="123"/>
-      <c r="B22" s="125"/>
-      <c r="C22" s="114"/>
+      <c r="A22" s="120"/>
+      <c r="B22" s="122"/>
+      <c r="C22" s="124"/>
       <c r="D22" s="15" t="s">
         <v>124</v>
       </c>
@@ -6898,9 +6898,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="123"/>
-      <c r="B23" s="125"/>
-      <c r="C23" s="114"/>
+      <c r="A23" s="120"/>
+      <c r="B23" s="122"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="15" t="s">
         <v>125</v>
       </c>
@@ -6909,9 +6909,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="123"/>
-      <c r="B24" s="125"/>
-      <c r="C24" s="114"/>
+      <c r="A24" s="120"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="124"/>
       <c r="D24" s="15" t="s">
         <v>126</v>
       </c>
@@ -6920,18 +6920,18 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="123"/>
-      <c r="B25" s="125"/>
-      <c r="C25" s="114"/>
+      <c r="A25" s="120"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="124"/>
       <c r="D25" s="15" t="s">
         <v>127</v>
       </c>
       <c r="E25" s="33"/>
     </row>
     <row r="26" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="123"/>
-      <c r="B26" s="125"/>
-      <c r="C26" s="114"/>
+      <c r="A26" s="120"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="124"/>
       <c r="D26" s="15" t="s">
         <v>128</v>
       </c>
@@ -6940,94 +6940,94 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="123"/>
-      <c r="B27" s="125"/>
-      <c r="C27" s="114"/>
+      <c r="A27" s="120"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="124"/>
       <c r="D27" s="15" t="s">
         <v>129</v>
       </c>
       <c r="E27" s="33"/>
     </row>
     <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="123"/>
-      <c r="B28" s="125"/>
-      <c r="C28" s="114"/>
+      <c r="A28" s="120"/>
+      <c r="B28" s="122"/>
+      <c r="C28" s="124"/>
       <c r="D28" s="15" t="s">
         <v>130</v>
       </c>
       <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="123"/>
-      <c r="B29" s="125"/>
-      <c r="C29" s="114"/>
+      <c r="A29" s="120"/>
+      <c r="B29" s="122"/>
+      <c r="C29" s="124"/>
       <c r="D29" s="15" t="s">
         <v>131</v>
       </c>
       <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="123"/>
-      <c r="B30" s="125"/>
-      <c r="C30" s="114"/>
+      <c r="A30" s="120"/>
+      <c r="B30" s="122"/>
+      <c r="C30" s="124"/>
       <c r="D30" s="15" t="s">
         <v>132</v>
       </c>
       <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="123"/>
-      <c r="B31" s="125"/>
-      <c r="C31" s="114"/>
+      <c r="A31" s="120"/>
+      <c r="B31" s="122"/>
+      <c r="C31" s="124"/>
       <c r="D31" s="15" t="s">
         <v>133</v>
       </c>
       <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="123"/>
-      <c r="B32" s="125"/>
-      <c r="C32" s="114"/>
+      <c r="A32" s="120"/>
+      <c r="B32" s="122"/>
+      <c r="C32" s="124"/>
       <c r="D32" s="15" t="s">
         <v>134</v>
       </c>
       <c r="E32" s="33"/>
     </row>
     <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="123"/>
-      <c r="B33" s="125"/>
-      <c r="C33" s="114"/>
+      <c r="A33" s="120"/>
+      <c r="B33" s="122"/>
+      <c r="C33" s="124"/>
       <c r="D33" s="15" t="s">
         <v>135</v>
       </c>
       <c r="E33" s="33"/>
     </row>
     <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="123"/>
-      <c r="B34" s="125"/>
-      <c r="C34" s="114"/>
+      <c r="A34" s="120"/>
+      <c r="B34" s="122"/>
+      <c r="C34" s="124"/>
       <c r="D34" s="15" t="s">
         <v>136</v>
       </c>
       <c r="E34" s="33"/>
     </row>
     <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="124"/>
-      <c r="B35" s="126"/>
-      <c r="C35" s="115"/>
+      <c r="A35" s="116"/>
+      <c r="B35" s="118"/>
+      <c r="C35" s="125"/>
       <c r="D35" s="16" t="s">
         <v>137</v>
       </c>
       <c r="E35" s="34"/>
     </row>
     <row r="36" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="116" t="s">
+      <c r="A36" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="113" t="s">
+      <c r="B36" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="123" t="s">
         <v>143</v>
       </c>
       <c r="D36" s="14" t="s">
@@ -7038,18 +7038,18 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="123"/>
-      <c r="B37" s="125"/>
-      <c r="C37" s="114"/>
+      <c r="A37" s="120"/>
+      <c r="B37" s="122"/>
+      <c r="C37" s="124"/>
       <c r="D37" s="15" t="s">
         <v>145</v>
       </c>
       <c r="E37" s="33"/>
     </row>
     <row r="38" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="123"/>
-      <c r="B38" s="125"/>
-      <c r="C38" s="114"/>
+      <c r="A38" s="120"/>
+      <c r="B38" s="122"/>
+      <c r="C38" s="124"/>
       <c r="D38" s="15" t="s">
         <v>146</v>
       </c>
@@ -7058,138 +7058,138 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="123"/>
-      <c r="B39" s="125"/>
-      <c r="C39" s="114"/>
+      <c r="A39" s="120"/>
+      <c r="B39" s="122"/>
+      <c r="C39" s="124"/>
       <c r="D39" s="15" t="s">
         <v>147</v>
       </c>
       <c r="E39" s="33"/>
     </row>
     <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="124"/>
-      <c r="B40" s="126"/>
-      <c r="C40" s="115"/>
+      <c r="A40" s="116"/>
+      <c r="B40" s="118"/>
+      <c r="C40" s="125"/>
       <c r="D40" s="16" t="s">
         <v>148</v>
       </c>
       <c r="E40" s="34"/>
     </row>
     <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="116" t="s">
+      <c r="A41" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="113" t="s">
+      <c r="B41" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="123" t="s">
         <v>151</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="E41" s="121"/>
+      <c r="E41" s="129"/>
     </row>
     <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="124"/>
-      <c r="B42" s="126"/>
-      <c r="C42" s="115"/>
+      <c r="A42" s="116"/>
+      <c r="B42" s="118"/>
+      <c r="C42" s="125"/>
       <c r="D42" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E42" s="130"/>
+      <c r="E42" s="131"/>
     </row>
     <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="116" t="s">
+      <c r="A43" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="113" t="s">
+      <c r="B43" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="123" t="s">
         <v>154</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="E43" s="121"/>
+      <c r="E43" s="129"/>
     </row>
     <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="124"/>
-      <c r="B44" s="126"/>
-      <c r="C44" s="115"/>
+      <c r="A44" s="116"/>
+      <c r="B44" s="118"/>
+      <c r="C44" s="125"/>
       <c r="D44" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="E44" s="130"/>
+      <c r="E44" s="131"/>
     </row>
     <row r="45" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="116" t="s">
+      <c r="A45" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="113" t="s">
+      <c r="B45" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="123" t="s">
         <v>157</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="E45" s="113" t="s">
+      <c r="E45" s="123" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="124"/>
-      <c r="B46" s="126"/>
-      <c r="C46" s="115"/>
+      <c r="A46" s="116"/>
+      <c r="B46" s="118"/>
+      <c r="C46" s="125"/>
       <c r="D46" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="E46" s="115"/>
+      <c r="E46" s="125"/>
     </row>
     <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="116" t="s">
+      <c r="A47" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="113" t="s">
+      <c r="B47" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="123" t="s">
         <v>161</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="127"/>
+      <c r="E47" s="126"/>
     </row>
     <row r="48" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="123"/>
-      <c r="B48" s="125"/>
-      <c r="C48" s="114"/>
+      <c r="A48" s="120"/>
+      <c r="B48" s="122"/>
+      <c r="C48" s="124"/>
       <c r="D48" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="E48" s="129"/>
+      <c r="E48" s="127"/>
     </row>
     <row r="49" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="123"/>
-      <c r="B49" s="125"/>
-      <c r="C49" s="114"/>
+      <c r="A49" s="120"/>
+      <c r="B49" s="122"/>
+      <c r="C49" s="124"/>
       <c r="D49" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="E49" s="129"/>
+      <c r="E49" s="127"/>
     </row>
     <row r="50" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="124"/>
-      <c r="B50" s="126"/>
-      <c r="C50" s="115"/>
+      <c r="A50" s="116"/>
+      <c r="B50" s="118"/>
+      <c r="C50" s="125"/>
       <c r="D50" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="E50" s="128"/>
+      <c r="E50" s="114"/>
     </row>
     <row r="51" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A51" s="132" t="s">
@@ -7242,13 +7242,13 @@
       <c r="E54" s="42"/>
     </row>
     <row r="55" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A55" s="116" t="s">
+      <c r="A55" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B55" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C55" s="113" t="s">
+      <c r="B55" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="123" t="s">
         <v>172</v>
       </c>
       <c r="D55" s="14" t="s">
@@ -7259,18 +7259,18 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="123"/>
-      <c r="B56" s="125"/>
-      <c r="C56" s="114"/>
+      <c r="A56" s="120"/>
+      <c r="B56" s="122"/>
+      <c r="C56" s="124"/>
       <c r="D56" s="15" t="s">
         <v>174</v>
       </c>
       <c r="E56" s="33"/>
     </row>
     <row r="57" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="123"/>
-      <c r="B57" s="125"/>
-      <c r="C57" s="114"/>
+      <c r="A57" s="120"/>
+      <c r="B57" s="122"/>
+      <c r="C57" s="124"/>
       <c r="D57" s="15" t="s">
         <v>175</v>
       </c>
@@ -7279,66 +7279,66 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="124"/>
-      <c r="B58" s="126"/>
-      <c r="C58" s="115"/>
+      <c r="A58" s="116"/>
+      <c r="B58" s="118"/>
+      <c r="C58" s="125"/>
       <c r="D58" s="16" t="s">
         <v>176</v>
       </c>
       <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="116" t="s">
+      <c r="A59" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B59" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C59" s="113" t="s">
+      <c r="B59" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C59" s="123" t="s">
         <v>179</v>
       </c>
       <c r="D59" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="E59" s="113" t="s">
+      <c r="E59" s="123" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="123"/>
-      <c r="B60" s="125"/>
-      <c r="C60" s="114"/>
+      <c r="A60" s="120"/>
+      <c r="B60" s="122"/>
+      <c r="C60" s="124"/>
       <c r="D60" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="E60" s="114"/>
+      <c r="E60" s="124"/>
     </row>
     <row r="61" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="123"/>
-      <c r="B61" s="125"/>
-      <c r="C61" s="114"/>
+      <c r="A61" s="120"/>
+      <c r="B61" s="122"/>
+      <c r="C61" s="124"/>
       <c r="D61" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="E61" s="114"/>
+      <c r="E61" s="124"/>
     </row>
     <row r="62" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="124"/>
-      <c r="B62" s="126"/>
-      <c r="C62" s="115"/>
+      <c r="A62" s="116"/>
+      <c r="B62" s="118"/>
+      <c r="C62" s="125"/>
       <c r="D62" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="E62" s="115"/>
+      <c r="E62" s="125"/>
     </row>
     <row r="63" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="116" t="s">
+      <c r="A63" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B63" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C63" s="113" t="s">
+      <c r="B63" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" s="123" t="s">
         <v>184</v>
       </c>
       <c r="D63" s="14" t="s">
@@ -7349,18 +7349,18 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="123"/>
-      <c r="B64" s="125"/>
-      <c r="C64" s="114"/>
+      <c r="A64" s="120"/>
+      <c r="B64" s="122"/>
+      <c r="C64" s="124"/>
       <c r="D64" s="15" t="s">
         <v>186</v>
       </c>
       <c r="E64" s="33"/>
     </row>
     <row r="65" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="123"/>
-      <c r="B65" s="125"/>
-      <c r="C65" s="114"/>
+      <c r="A65" s="120"/>
+      <c r="B65" s="122"/>
+      <c r="C65" s="124"/>
       <c r="D65" s="15" t="s">
         <v>187</v>
       </c>
@@ -7369,18 +7369,18 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="123"/>
-      <c r="B66" s="125"/>
-      <c r="C66" s="114"/>
+      <c r="A66" s="120"/>
+      <c r="B66" s="122"/>
+      <c r="C66" s="124"/>
       <c r="D66" s="15" t="s">
         <v>188</v>
       </c>
       <c r="E66" s="33"/>
     </row>
     <row r="67" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="123"/>
-      <c r="B67" s="125"/>
-      <c r="C67" s="114"/>
+      <c r="A67" s="120"/>
+      <c r="B67" s="122"/>
+      <c r="C67" s="124"/>
       <c r="D67" s="15" t="s">
         <v>189</v>
       </c>
@@ -7389,84 +7389,84 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="123"/>
-      <c r="B68" s="125"/>
-      <c r="C68" s="114"/>
+      <c r="A68" s="120"/>
+      <c r="B68" s="122"/>
+      <c r="C68" s="124"/>
       <c r="D68" s="15" t="s">
         <v>190</v>
       </c>
       <c r="E68" s="33"/>
     </row>
     <row r="69" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="123"/>
-      <c r="B69" s="125"/>
-      <c r="C69" s="114"/>
+      <c r="A69" s="120"/>
+      <c r="B69" s="122"/>
+      <c r="C69" s="124"/>
       <c r="D69" s="15" t="s">
         <v>191</v>
       </c>
       <c r="E69" s="33"/>
     </row>
     <row r="70" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="124"/>
-      <c r="B70" s="126"/>
-      <c r="C70" s="115"/>
+      <c r="A70" s="116"/>
+      <c r="B70" s="118"/>
+      <c r="C70" s="125"/>
       <c r="D70" s="16" t="s">
         <v>192</v>
       </c>
       <c r="E70" s="34"/>
     </row>
     <row r="71" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="116" t="s">
+      <c r="A71" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B71" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C71" s="113" t="s">
+      <c r="B71" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71" s="123" t="s">
         <v>196</v>
       </c>
       <c r="D71" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="E71" s="113" t="s">
+      <c r="E71" s="123" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="123"/>
-      <c r="B72" s="125"/>
-      <c r="C72" s="114"/>
+      <c r="A72" s="120"/>
+      <c r="B72" s="122"/>
+      <c r="C72" s="124"/>
       <c r="D72" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="E72" s="114"/>
+      <c r="E72" s="124"/>
     </row>
     <row r="73" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="123"/>
-      <c r="B73" s="125"/>
-      <c r="C73" s="114"/>
+      <c r="A73" s="120"/>
+      <c r="B73" s="122"/>
+      <c r="C73" s="124"/>
       <c r="D73" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="E73" s="114"/>
+      <c r="E73" s="124"/>
     </row>
     <row r="74" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="124"/>
-      <c r="B74" s="126"/>
-      <c r="C74" s="115"/>
+      <c r="A74" s="116"/>
+      <c r="B74" s="118"/>
+      <c r="C74" s="125"/>
       <c r="D74" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="E74" s="115"/>
+      <c r="E74" s="125"/>
     </row>
     <row r="75" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="116" t="s">
+      <c r="A75" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B75" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C75" s="113" t="s">
+      <c r="B75" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C75" s="123" t="s">
         <v>202</v>
       </c>
       <c r="D75" s="43" t="s">
@@ -7477,9 +7477,9 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="123"/>
-      <c r="B76" s="125"/>
-      <c r="C76" s="114"/>
+      <c r="A76" s="120"/>
+      <c r="B76" s="122"/>
+      <c r="C76" s="124"/>
       <c r="D76" s="15" t="s">
         <v>204</v>
       </c>
@@ -7488,31 +7488,31 @@
       </c>
     </row>
     <row r="77" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="123"/>
-      <c r="B77" s="125"/>
-      <c r="C77" s="114"/>
+      <c r="A77" s="120"/>
+      <c r="B77" s="122"/>
+      <c r="C77" s="124"/>
       <c r="D77" s="15" t="s">
         <v>205</v>
       </c>
       <c r="E77" s="33"/>
     </row>
     <row r="78" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="124"/>
-      <c r="B78" s="126"/>
-      <c r="C78" s="115"/>
+      <c r="A78" s="116"/>
+      <c r="B78" s="118"/>
+      <c r="C78" s="125"/>
       <c r="D78" s="16" t="s">
         <v>206</v>
       </c>
       <c r="E78" s="34"/>
     </row>
     <row r="79" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A79" s="116" t="s">
+      <c r="A79" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B79" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C79" s="113" t="s">
+      <c r="B79" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C79" s="123" t="s">
         <v>209</v>
       </c>
       <c r="D79" s="14" t="s">
@@ -7523,18 +7523,18 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="123"/>
-      <c r="B80" s="125"/>
-      <c r="C80" s="114"/>
+      <c r="A80" s="120"/>
+      <c r="B80" s="122"/>
+      <c r="C80" s="124"/>
       <c r="D80" s="15" t="s">
         <v>211</v>
       </c>
       <c r="E80" s="33"/>
     </row>
     <row r="81" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A81" s="123"/>
-      <c r="B81" s="125"/>
-      <c r="C81" s="114"/>
+      <c r="A81" s="120"/>
+      <c r="B81" s="122"/>
+      <c r="C81" s="124"/>
       <c r="D81" s="15" t="s">
         <v>212</v>
       </c>
@@ -7543,27 +7543,27 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="123"/>
-      <c r="B82" s="125"/>
-      <c r="C82" s="114"/>
+      <c r="A82" s="120"/>
+      <c r="B82" s="122"/>
+      <c r="C82" s="124"/>
       <c r="D82" s="15" t="s">
         <v>213</v>
       </c>
       <c r="E82" s="33"/>
     </row>
     <row r="83" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="123"/>
-      <c r="B83" s="125"/>
-      <c r="C83" s="114"/>
+      <c r="A83" s="120"/>
+      <c r="B83" s="122"/>
+      <c r="C83" s="124"/>
       <c r="D83" s="15" t="s">
         <v>214</v>
       </c>
       <c r="E83" s="33"/>
     </row>
     <row r="84" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="124"/>
-      <c r="B84" s="126"/>
-      <c r="C84" s="115"/>
+      <c r="A84" s="116"/>
+      <c r="B84" s="118"/>
+      <c r="C84" s="125"/>
       <c r="D84" s="16" t="s">
         <v>215</v>
       </c>
@@ -7602,55 +7602,55 @@
       <c r="E86" s="42"/>
     </row>
     <row r="87" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A87" s="116" t="s">
+      <c r="A87" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B87" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C87" s="113" t="s">
+      <c r="B87" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87" s="123" t="s">
         <v>222</v>
       </c>
       <c r="D87" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="E87" s="127"/>
+      <c r="E87" s="126"/>
     </row>
     <row r="88" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="123"/>
-      <c r="B88" s="125"/>
-      <c r="C88" s="114"/>
+      <c r="A88" s="120"/>
+      <c r="B88" s="122"/>
+      <c r="C88" s="124"/>
       <c r="D88" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="E88" s="129"/>
+      <c r="E88" s="127"/>
     </row>
     <row r="89" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="123"/>
-      <c r="B89" s="125"/>
-      <c r="C89" s="114"/>
+      <c r="A89" s="120"/>
+      <c r="B89" s="122"/>
+      <c r="C89" s="124"/>
       <c r="D89" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="E89" s="129"/>
+      <c r="E89" s="127"/>
     </row>
     <row r="90" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="123"/>
-      <c r="B90" s="125"/>
-      <c r="C90" s="114"/>
+      <c r="A90" s="120"/>
+      <c r="B90" s="122"/>
+      <c r="C90" s="124"/>
       <c r="D90" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="E90" s="129"/>
+      <c r="E90" s="127"/>
     </row>
     <row r="91" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="124"/>
-      <c r="B91" s="126"/>
-      <c r="C91" s="115"/>
+      <c r="A91" s="116"/>
+      <c r="B91" s="118"/>
+      <c r="C91" s="125"/>
       <c r="D91" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="E91" s="128"/>
+      <c r="E91" s="114"/>
     </row>
     <row r="92" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="44" t="s">
@@ -7702,87 +7702,87 @@
       <c r="E94" s="46"/>
     </row>
     <row r="95" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="116" t="s">
+      <c r="A95" s="119" t="s">
         <v>234</v>
       </c>
-      <c r="B95" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C95" s="113" t="s">
+      <c r="B95" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C95" s="123" t="s">
         <v>237</v>
       </c>
       <c r="D95" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="E95" s="127"/>
+      <c r="E95" s="126"/>
     </row>
     <row r="96" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="124"/>
-      <c r="B96" s="126"/>
-      <c r="C96" s="115"/>
+      <c r="A96" s="116"/>
+      <c r="B96" s="118"/>
+      <c r="C96" s="125"/>
       <c r="D96" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="E96" s="128"/>
+      <c r="E96" s="114"/>
     </row>
     <row r="97" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="116" t="s">
+      <c r="A97" s="119" t="s">
         <v>234</v>
       </c>
-      <c r="B97" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C97" s="113" t="s">
+      <c r="B97" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C97" s="123" t="s">
         <v>240</v>
       </c>
       <c r="D97" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="E97" s="127"/>
+      <c r="E97" s="126"/>
     </row>
     <row r="98" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="124"/>
-      <c r="B98" s="126"/>
-      <c r="C98" s="115"/>
+      <c r="A98" s="116"/>
+      <c r="B98" s="118"/>
+      <c r="C98" s="125"/>
       <c r="D98" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="E98" s="128"/>
+      <c r="E98" s="114"/>
     </row>
     <row r="99" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="116" t="s">
+      <c r="A99" s="119" t="s">
         <v>234</v>
       </c>
-      <c r="B99" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C99" s="113" t="s">
+      <c r="B99" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C99" s="123" t="s">
         <v>242</v>
       </c>
       <c r="D99" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E99" s="113" t="s">
+      <c r="E99" s="123" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="123"/>
-      <c r="B100" s="125"/>
-      <c r="C100" s="114"/>
+      <c r="A100" s="120"/>
+      <c r="B100" s="122"/>
+      <c r="C100" s="124"/>
       <c r="D100" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="E100" s="114"/>
+      <c r="E100" s="124"/>
     </row>
     <row r="101" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="124"/>
-      <c r="B101" s="126"/>
-      <c r="C101" s="115"/>
+      <c r="A101" s="116"/>
+      <c r="B101" s="118"/>
+      <c r="C101" s="125"/>
       <c r="D101" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="E101" s="115"/>
+      <c r="E101" s="125"/>
     </row>
     <row r="102" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="47" t="s">
@@ -7802,85 +7802,141 @@
       </c>
     </row>
     <row r="103" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="116" t="s">
+      <c r="A103" s="119" t="s">
         <v>234</v>
       </c>
-      <c r="B103" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C103" s="113" t="s">
+      <c r="B103" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C103" s="123" t="s">
         <v>248</v>
       </c>
       <c r="D103" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E103" s="113" t="s">
+      <c r="E103" s="123" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="123"/>
-      <c r="B104" s="125"/>
-      <c r="C104" s="114"/>
+      <c r="A104" s="120"/>
+      <c r="B104" s="122"/>
+      <c r="C104" s="124"/>
       <c r="D104" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E104" s="114"/>
+      <c r="E104" s="124"/>
     </row>
     <row r="105" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="124"/>
-      <c r="B105" s="126"/>
-      <c r="C105" s="115"/>
+      <c r="A105" s="116"/>
+      <c r="B105" s="118"/>
+      <c r="C105" s="125"/>
       <c r="D105" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="E105" s="115"/>
+      <c r="E105" s="125"/>
     </row>
     <row r="106" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="116" t="s">
+      <c r="A106" s="119" t="s">
         <v>234</v>
       </c>
-      <c r="B106" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C106" s="113" t="s">
+      <c r="B106" s="121" t="s">
+        <v>91</v>
+      </c>
+      <c r="C106" s="123" t="s">
         <v>251</v>
       </c>
       <c r="D106" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="E106" s="121"/>
+      <c r="E106" s="129"/>
     </row>
     <row r="107" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="117"/>
-      <c r="B107" s="119"/>
-      <c r="C107" s="120"/>
+      <c r="A107" s="141"/>
+      <c r="B107" s="142"/>
+      <c r="C107" s="143"/>
       <c r="D107" s="50" t="s">
         <v>224</v>
       </c>
-      <c r="E107" s="122"/>
+      <c r="E107" s="144"/>
+    </row>
+    <row r="108" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="119"/>
+      <c r="B108" s="121"/>
+      <c r="C108" s="123"/>
+      <c r="D108" s="14"/>
+      <c r="E108" s="129"/>
+    </row>
+    <row r="109" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="141"/>
+      <c r="B109" s="142"/>
+      <c r="C109" s="143"/>
+      <c r="D109" s="50"/>
+      <c r="E109" s="144"/>
     </row>
   </sheetData>
-  <mergeCells count="92">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E87:E91"/>
-    <mergeCell ref="B79:B84"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="C95:C96"/>
-    <mergeCell ref="C75:C78"/>
-    <mergeCell ref="A79:A84"/>
-    <mergeCell ref="C79:C84"/>
-    <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="C87:C91"/>
+  <mergeCells count="96">
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="E103:E105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="B106:B107"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="B103:B105"/>
+    <mergeCell ref="E97:E98"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="E99:E101"/>
+    <mergeCell ref="C103:C105"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A63:A70"/>
+    <mergeCell ref="B63:B70"/>
+    <mergeCell ref="C63:C70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="A21:A35"/>
+    <mergeCell ref="B21:B35"/>
+    <mergeCell ref="C21:C35"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
     <mergeCell ref="C97:C98"/>
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="A43:A44"/>
@@ -7897,63 +7953,25 @@
     <mergeCell ref="E95:E96"/>
     <mergeCell ref="A75:A78"/>
     <mergeCell ref="B75:B78"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A21:A35"/>
-    <mergeCell ref="B21:B35"/>
-    <mergeCell ref="C21:C35"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="A63:A70"/>
-    <mergeCell ref="B63:B70"/>
-    <mergeCell ref="C63:C70"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="E71:E74"/>
-    <mergeCell ref="E103:E105"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="B106:B107"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="B103:B105"/>
-    <mergeCell ref="E97:E98"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="E99:E101"/>
-    <mergeCell ref="C103:C105"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="A79:A84"/>
+    <mergeCell ref="C79:C84"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="E87:E91"/>
+    <mergeCell ref="B79:B84"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>